<commit_message>
A course on Spatial Data Science
</commit_message>
<xml_diff>
--- a/tables/courses.xlsx
+++ b/tables/courses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/materov/ALL/@GitProjects/@2024/rsources-book/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EBFAB6-BC52-A145-926F-5EF9BF947BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007FA3D0-4E5D-C248-B92E-422805CC9233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="500" windowWidth="24940" windowHeight="14180" xr2:uid="{5BDCF2DE-D288-8A47-93F2-1E601DE6F859}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="145">
   <si>
     <t>author</t>
   </si>
@@ -464,6 +464,12 @@
   </si>
   <si>
     <t>Tiffany A. Timbers, Joel Ostblom, Florencia D’Andrea, Rodolfo Lourenzutti, Daniel Chen</t>
+  </si>
+  <si>
+    <t>A course on Spatial Data Science for Social Geography</t>
+  </si>
+  <si>
+    <t>https://martinfleischmann.net/sds/micro/</t>
   </si>
 </sst>
 </file>
@@ -819,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B785E614-6E2E-D84F-9372-795F7ED904A9}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1286,7 +1292,7 @@
         <v>70</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>69</v>
@@ -1295,57 +1301,57 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>79</v>
+        <v>144</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>38</v>
@@ -1353,13 +1359,13 @@
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>38</v>
@@ -1367,41 +1373,41 @@
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>45</v>
+        <v>125</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>44</v>
+        <v>126</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>43</v>
+        <v>124</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>42</v>
@@ -1409,13 +1415,13 @@
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>42</v>
@@ -1423,27 +1429,27 @@
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>42</v>
@@ -1451,44 +1457,44 @@
     </row>
     <row r="45" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1496,26 +1502,40 @@
         <v>93</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>